<commit_message>
Versión mas reciente del codigo
</commit_message>
<xml_diff>
--- a/BASES LIDE/cf_selected_4.xlsx
+++ b/BASES LIDE/cf_selected_4.xlsx
@@ -1,55 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Git hub\Confianza\BASES LIDE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">ano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_cf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_gob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_otra_reg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_police</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sierra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Costa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>Sierra</t>
+  </si>
+  <si>
+    <t>Costa</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>confianza Familia</t>
+  </si>
+  <si>
+    <t>Confianza Gobierno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confianza en Personas de otras Regiones </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confianza Policía </t>
+  </si>
+  <si>
+    <t>Región</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -78,13 +90,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -366,115 +393,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="2">
+        <v>0.94324853228962802</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.54011741682974601</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.37573385518591002</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.48923679060665398</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C3" s="2">
+        <v>0.94505494505494503</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.46781789638932503</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.32182103610675</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.45839874411303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.86744639376218302</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.321637426900585</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.216374269005848</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.573099415204678</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.943248532289628</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.540117416829746</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.37573385518591</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.489236790606654</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.81632653061224503</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.30612244897959201</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.19623233908948201</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.48665620094191497</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.945054945054945</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.467817896389325</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.32182103610675</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.45839874411303</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.867446393762183</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.321637426900585</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.216374269005848</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.573099415204678</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.816326530612245</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.306122448979592</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.196232339089482</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.486656200941915</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>